<commit_message>
Adapting for Ramp up
</commit_message>
<xml_diff>
--- a/runs.xlsx
+++ b/runs.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Documents\GitHub\241165\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B56A58-56FA-4CC5-9B45-F53017558CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2224F5EE-B0F8-465C-A141-63D34F0EC439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1962" yWindow="1746" windowWidth="17172" windowHeight="9936" xr2:uid="{88C63FDF-66B9-42B3-9B5D-45766DF4CCDF}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="2" xr2:uid="{88C63FDF-66B9-42B3-9B5D-45766DF4CCDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>File</t>
   </si>
@@ -48,6 +50,18 @@
   </si>
   <si>
     <t>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py</t>
+  </si>
+  <si>
+    <t>source /home/stimsim/Documents/241165/neusin/bin/activate</t>
+  </si>
+  <si>
+    <t>python3</t>
+  </si>
+  <si>
+    <t>/home/stimsim/Documents/241165/run_batch.py</t>
+  </si>
+  <si>
+    <t>modfreq</t>
   </si>
 </sst>
 </file>
@@ -419,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFDEEEE-9C87-4F42-BB66-64366C879522}">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -446,1552 +460,3574 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2" t="str">
-        <f>$A$2 &amp; " -f " &amp; B2 &amp; " -v " &amp; C2 &amp; " &gt;&gt; logs\" &amp; B2 &amp; ".log 2&gt;&amp;1"</f>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 10 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <f t="shared" ref="D2:D33" si="0">$A$2 &amp; " -f " &amp; B2 &amp; " -v " &amp; C2 &amp; " &gt;&gt; logs\" &amp; B2 &amp; ".log 2&gt;&amp;1"</f>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 10 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B3">
-        <f>B2</f>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D66" si="0">$A$2 &amp; " -f " &amp; B3 &amp; " -v " &amp; C3 &amp; " &gt;&gt; logs\" &amp; B3 &amp; ".log 2&gt;&amp;1"</f>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 20 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <f t="shared" si="0"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 20 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4">
-        <f>B3</f>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C4">
         <v>30</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 30 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 30 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
-        <f t="shared" ref="B5:B56" si="1">B4</f>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C5">
         <v>50</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 50 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 50 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B6">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C6">
         <v>100</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 100 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 100 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B7">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <v>150</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 150 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 150 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C8">
         <v>200</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 200 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 200 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C9">
         <v>300</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 300 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 300 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C10">
         <v>400</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 400 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 400 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C11">
         <v>500</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 500 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 500 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C12">
         <v>700</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 700 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 700 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B13">
-        <f t="shared" si="1"/>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C13">
         <v>1000</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 1000 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 200 -v 1000 &gt;&gt; logs\200.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B14">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 10 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 10 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B15">
-        <f t="shared" si="1"/>
-        <v>1000</v>
+        <f>B14</f>
+        <v>500</v>
       </c>
       <c r="C15">
         <v>20</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 20 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 20 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B16">
-        <f t="shared" si="1"/>
-        <v>1000</v>
+        <f>B15</f>
+        <v>500</v>
       </c>
       <c r="C16">
         <v>30</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 30 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 30 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17">
-        <f t="shared" si="1"/>
-        <v>1000</v>
+        <f t="shared" ref="B17:B68" si="1">B16</f>
+        <v>500</v>
       </c>
       <c r="C17">
         <v>50</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 50 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 50 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B18">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C18">
         <v>100</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 100 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 100 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B19">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C19">
         <v>150</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 150 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 150 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B20">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C20">
         <v>200</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 200 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 200 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B21">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C21">
         <v>300</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 300 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 300 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C22">
         <v>400</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 400 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 400 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B23">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C23">
         <v>500</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 500 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 500 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B24">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C24">
         <v>700</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 700 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 700 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B25">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C25">
         <v>1000</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 1000 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 500 -v 1000 &gt;&gt; logs\500.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B26">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C26">
         <v>10</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 10 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 10 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B27">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C27">
         <v>20</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 20 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 20 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B28">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C28">
         <v>30</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 30 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 30 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B29">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C29">
         <v>50</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 50 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 50 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B30">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C30">
         <v>100</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 100 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 100 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B31">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C31">
         <v>150</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 150 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 150 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B32">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C32">
         <v>200</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 200 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 200 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B33">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C33">
         <v>300</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 300 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 300 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B34">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C34">
         <v>400</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 400 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <f t="shared" ref="D34:D65" si="2">$A$2 &amp; " -f " &amp; B34 &amp; " -v " &amp; C34 &amp; " &gt;&gt; logs\" &amp; B34 &amp; ".log 2&gt;&amp;1"</f>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 400 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B35">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C35">
         <v>500</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 500 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 500 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B36">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C36">
         <v>700</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 700 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 700 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B37">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C37">
         <v>1000</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 1000 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 1000 -v 1000 &gt;&gt; logs\1000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B38">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C38">
         <v>10</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 10 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 10 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B39">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C39">
         <v>20</v>
       </c>
       <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 20 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 20 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B40">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C40">
         <v>30</v>
       </c>
       <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 30 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 30 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B41">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C41">
         <v>50</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 50 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 50 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B42">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C42">
         <v>100</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 100 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 100 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B43">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C43">
         <v>150</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 150 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 150 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B44">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C44">
         <v>200</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 200 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 200 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B45">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C45">
         <v>300</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 300 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 300 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B46">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C46">
         <v>400</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 400 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 400 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B47">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C47">
         <v>500</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 500 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 500 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B48">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C48">
         <v>700</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 700 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 700 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B49">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C49">
         <v>1000</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 1000 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 2000 -v 1000 &gt;&gt; logs\2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B50">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C50">
         <v>10</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 10 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 10 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B51">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C51">
         <v>20</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 20 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 20 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B52">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C52">
         <v>30</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 30 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 30 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B53">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C53">
         <v>50</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 50 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 50 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B54">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C54">
         <v>100</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 100 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 100 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B55">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C55">
         <v>150</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 150 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 150 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B56">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C56">
         <v>200</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 200 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 200 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B57">
-        <f t="shared" ref="B57:B120" si="2">B56</f>
-        <v>5000</v>
+        <f t="shared" si="1"/>
+        <v>3000</v>
       </c>
       <c r="C57">
         <v>300</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 300 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 300 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B58">
-        <f t="shared" si="2"/>
-        <v>5000</v>
+        <f t="shared" si="1"/>
+        <v>3000</v>
       </c>
       <c r="C58">
         <v>400</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 400 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 400 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B59">
-        <f t="shared" si="2"/>
-        <v>5000</v>
+        <f t="shared" si="1"/>
+        <v>3000</v>
       </c>
       <c r="C59">
         <v>500</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 500 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 500 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B60">
-        <f t="shared" si="2"/>
-        <v>5000</v>
+        <f t="shared" si="1"/>
+        <v>3000</v>
       </c>
       <c r="C60">
         <v>700</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 700 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 700 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B61">
-        <f t="shared" si="2"/>
-        <v>5000</v>
+        <f t="shared" si="1"/>
+        <v>3000</v>
       </c>
       <c r="C61">
         <v>1000</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 1000 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 3000 -v 1000 &gt;&gt; logs\3000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B62">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="C62">
         <v>10</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 10 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 10 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B63">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" si="1"/>
+        <v>5000</v>
       </c>
       <c r="C63">
         <v>20</v>
       </c>
       <c r="D63" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 20 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 20 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B64">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" si="1"/>
+        <v>5000</v>
       </c>
       <c r="C64">
         <v>30</v>
       </c>
       <c r="D64" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 30 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 30 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B65">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" si="1"/>
+        <v>5000</v>
       </c>
       <c r="C65">
         <v>50</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 50 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 50 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B66">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" si="1"/>
+        <v>5000</v>
       </c>
       <c r="C66">
         <v>100</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="0"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 100 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <f t="shared" ref="D66:D97" si="3">$A$2 &amp; " -f " &amp; B66 &amp; " -v " &amp; C66 &amp; " &gt;&gt; logs\" &amp; B66 &amp; ".log 2&gt;&amp;1"</f>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 100 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B67">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" si="1"/>
+        <v>5000</v>
       </c>
       <c r="C67">
         <v>150</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D121" si="3">$A$2 &amp; " -f " &amp; B67 &amp; " -v " &amp; C67 &amp; " &gt;&gt; logs\" &amp; B67 &amp; ".log 2&gt;&amp;1"</f>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 150 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <f t="shared" si="3"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 150 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B68">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" si="1"/>
+        <v>5000</v>
       </c>
       <c r="C68">
         <v>200</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 200 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 200 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B69">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" ref="B69:B132" si="4">B68</f>
+        <v>5000</v>
       </c>
       <c r="C69">
         <v>300</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 300 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 300 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B70">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" si="4"/>
+        <v>5000</v>
       </c>
       <c r="C70">
         <v>400</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 400 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 400 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B71">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" si="4"/>
+        <v>5000</v>
       </c>
       <c r="C71">
         <v>500</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 500 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 500 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B72">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" si="4"/>
+        <v>5000</v>
       </c>
       <c r="C72">
         <v>700</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 700 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 700 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B73">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" si="4"/>
+        <v>5000</v>
       </c>
       <c r="C73">
         <v>1000</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 1000 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 5000 -v 1000 &gt;&gt; logs\5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B74">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="C74">
         <v>10</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 10 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 10 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B75">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C75">
         <v>20</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 20 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 20 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B76">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C76">
         <v>30</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 30 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 30 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B77">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C77">
         <v>50</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 50 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 50 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B78">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C78">
         <v>100</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 100 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 100 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B79">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C79">
         <v>150</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 150 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 150 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B80">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C80">
         <v>200</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 200 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 200 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B81">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C81">
         <v>300</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 300 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 300 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B82">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C82">
         <v>400</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 400 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 400 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B83">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C83">
         <v>500</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 500 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 500 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B84">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C84">
         <v>700</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 700 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 700 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B85">
-        <f t="shared" si="2"/>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="C85">
         <v>1000</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 1000 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 10000 -v 1000 &gt;&gt; logs\10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B86">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C86">
         <v>10</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 10 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 10 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B87">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C87">
         <v>20</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 20 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 20 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B88">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C88">
         <v>30</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 30 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 30 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B89">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C89">
         <v>50</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 50 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 50 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B90">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C90">
         <v>100</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 100 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 100 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B91">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C91">
         <v>150</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 150 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 150 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B92">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C92">
         <v>200</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 200 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 200 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B93">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C93">
         <v>300</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 300 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 300 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B94">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C94">
         <v>400</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 400 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 400 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B95">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C95">
         <v>500</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 500 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 500 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B96">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C96">
         <v>700</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 700 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 700 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B97">
-        <f t="shared" si="2"/>
-        <v>30000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="C97">
         <v>1000</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 1000 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 20000 -v 1000 &gt;&gt; logs\20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B98">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C98">
         <v>10</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 10 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" ref="D98:D129" si="5">$A$2 &amp; " -f " &amp; B98 &amp; " -v " &amp; C98 &amp; " &gt;&gt; logs\" &amp; B98 &amp; ".log 2&gt;&amp;1"</f>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 10 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B99">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C99">
         <v>20</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 20 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 20 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B100">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C100">
         <v>30</v>
       </c>
       <c r="D100" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 30 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 30 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B101">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C101">
         <v>50</v>
       </c>
       <c r="D101" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 50 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 50 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B102">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C102">
         <v>100</v>
       </c>
       <c r="D102" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 100 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 100 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B103">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C103">
         <v>150</v>
       </c>
       <c r="D103" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 150 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 150 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B104">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C104">
         <v>200</v>
       </c>
       <c r="D104" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 200 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 200 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B105">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C105">
         <v>300</v>
       </c>
       <c r="D105" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 300 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 300 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B106">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C106">
         <v>400</v>
       </c>
       <c r="D106" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 400 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 400 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B107">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C107">
         <v>500</v>
       </c>
       <c r="D107" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 500 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 500 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B108">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C108">
         <v>700</v>
       </c>
       <c r="D108" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 700 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 700 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B109">
-        <f t="shared" si="2"/>
-        <v>40000</v>
+        <f t="shared" si="4"/>
+        <v>30000</v>
       </c>
       <c r="C109">
         <v>1000</v>
       </c>
       <c r="D109" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 1000 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 30000 -v 1000 &gt;&gt; logs\30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B110">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C110">
         <v>10</v>
       </c>
       <c r="D110" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 10 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 10 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B111">
-        <f t="shared" si="2"/>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>40000</v>
       </c>
       <c r="C111">
         <v>20</v>
       </c>
       <c r="D111" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 20 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 20 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B112">
-        <f t="shared" si="2"/>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>40000</v>
       </c>
       <c r="C112">
         <v>30</v>
       </c>
       <c r="D112" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 30 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 30 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B113">
-        <f t="shared" si="2"/>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>40000</v>
       </c>
       <c r="C113">
         <v>50</v>
       </c>
       <c r="D113" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 50 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 50 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B114">
-        <f t="shared" si="2"/>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>40000</v>
       </c>
       <c r="C114">
         <v>100</v>
       </c>
       <c r="D114" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 100 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 100 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B115">
-        <f t="shared" si="2"/>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>40000</v>
       </c>
       <c r="C115">
         <v>150</v>
       </c>
       <c r="D115" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 150 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 150 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B116">
-        <f t="shared" si="2"/>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>40000</v>
       </c>
       <c r="C116">
         <v>200</v>
       </c>
       <c r="D116" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 200 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 200 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B117">
-        <f t="shared" si="2"/>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>40000</v>
       </c>
       <c r="C117">
         <v>300</v>
       </c>
       <c r="D117" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 300 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 300 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B118">
-        <f t="shared" si="2"/>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>40000</v>
       </c>
       <c r="C118">
         <v>400</v>
       </c>
       <c r="D118" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 400 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 400 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B119">
-        <f t="shared" si="2"/>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>40000</v>
       </c>
       <c r="C119">
         <v>500</v>
       </c>
       <c r="D119" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 500 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 500 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B120">
-        <f t="shared" si="2"/>
-        <v>50000</v>
+        <f t="shared" si="4"/>
+        <v>40000</v>
       </c>
       <c r="C120">
         <v>700</v>
       </c>
       <c r="D120" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 700 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 700 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B121">
-        <f t="shared" ref="B121" si="4">B120</f>
+        <f t="shared" si="4"/>
+        <v>40000</v>
+      </c>
+      <c r="C121">
+        <v>1000</v>
+      </c>
+      <c r="D121" t="str">
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 40000 -v 1000 &gt;&gt; logs\40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B122">
         <v>50000</v>
       </c>
+      <c r="C122">
+        <v>10</v>
+      </c>
+      <c r="D122" t="str">
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 10 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B123">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="C123">
+        <v>20</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 20 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B124">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="C124">
+        <v>30</v>
+      </c>
+      <c r="D124" t="str">
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 30 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B125">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="C125">
+        <v>50</v>
+      </c>
+      <c r="D125" t="str">
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 50 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B126">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="C126">
+        <v>100</v>
+      </c>
+      <c r="D126" t="str">
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 100 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B127">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="C127">
+        <v>150</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 150 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B128">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="C128">
+        <v>200</v>
+      </c>
+      <c r="D128" t="str">
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 200 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B129">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="C129">
+        <v>300</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="5"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 300 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B130">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="C130">
+        <v>400</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" ref="D130:D161" si="6">$A$2 &amp; " -f " &amp; B130 &amp; " -v " &amp; C130 &amp; " &gt;&gt; logs\" &amp; B130 &amp; ".log 2&gt;&amp;1"</f>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 400 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B131">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="C131">
+        <v>500</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" si="6"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 500 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B132">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="C132">
+        <v>700</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="6"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 700 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B133">
+        <f t="shared" ref="B133" si="7">B132</f>
+        <v>50000</v>
+      </c>
+      <c r="C133">
+        <v>1000</v>
+      </c>
+      <c r="D133" t="str">
+        <f t="shared" si="6"/>
+        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 1000 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0855CE45-A230-43B4-BABA-3BDF38256F68}">
+  <dimension ref="A1:S133"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="8.62890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="str">
+        <f>$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B2 &amp; " -v " &amp; C2 &amp; " &gt;&gt; logs/" &amp; B2 &amp; ".log 2&gt;&amp;1"</f>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 10 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D66" si="0">$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B3 &amp; " -v " &amp; C3 &amp; " &gt;&gt; logs/" &amp; B3 &amp; ".log 2&gt;&amp;1"</f>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 20 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 30 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5">
+        <v>200</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 50 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6">
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 100 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7">
+        <v>200</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 150 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="C8">
+        <v>200</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 200 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
+        <v>300</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 300 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10">
+        <v>400</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 400 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11">
+        <v>200</v>
+      </c>
+      <c r="C11">
+        <v>500</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 500 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12">
+        <v>200</v>
+      </c>
+      <c r="C12">
+        <v>700</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 700 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13">
+        <v>200</v>
+      </c>
+      <c r="C13">
+        <v>1000</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 200 -v 1000 &gt;&gt; logs/200.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14">
+        <v>500</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 10 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15">
+        <f>B14</f>
+        <v>500</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 20 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16">
+        <f>B15</f>
+        <v>500</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 30 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17">
+        <f t="shared" ref="B17:B80" si="1">B16</f>
+        <v>500</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 50 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 100 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="C19">
+        <v>150</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 150 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="C20">
+        <v>200</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 200 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="C21">
+        <v>300</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 300 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="C22">
+        <v>400</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 400 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="C23">
+        <v>500</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 500 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="C24">
+        <v>700</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 700 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="C25">
+        <v>1000</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 500 -v 1000 &gt;&gt; logs/500.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26">
+        <v>1000</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 10 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 20 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C28">
+        <v>30</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 30 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C29">
+        <v>50</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 50 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C30">
+        <v>100</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 100 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C31">
+        <v>150</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 150 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C32">
+        <v>200</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 200 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C33">
+        <v>300</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 300 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C34">
+        <v>400</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 400 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C35">
+        <v>500</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 500 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C36">
+        <v>700</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 700 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="C37">
+        <v>1000</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 1000 -v 1000 &gt;&gt; logs/1000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38">
+        <v>2000</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 10 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C39">
+        <v>20</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 20 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C40">
+        <v>30</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 30 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C41">
+        <v>50</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 50 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C42">
+        <v>100</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 100 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C43">
+        <v>150</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 150 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C44">
+        <v>200</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 200 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C45">
+        <v>300</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 300 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C46">
+        <v>400</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 400 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C47">
+        <v>500</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 500 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C48">
+        <v>700</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 700 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="C49">
+        <v>1000</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 1000 &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50">
+        <v>3000</v>
+      </c>
+      <c r="C50">
+        <v>10</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 10 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C51">
+        <v>20</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 20 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C52">
+        <v>30</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 30 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C53">
+        <v>50</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 50 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C54">
+        <v>100</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 100 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C55">
+        <v>150</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 150 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C56">
+        <v>200</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 200 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C57">
+        <v>300</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 300 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C58">
+        <v>400</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 400 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C59">
+        <v>500</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 500 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C60">
+        <v>700</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 700 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B61">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C61">
+        <v>1000</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 3000 -v 1000 &gt;&gt; logs/3000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62">
+        <v>5000</v>
+      </c>
+      <c r="C62">
+        <v>10</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 10 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B63">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C63">
+        <v>20</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 20 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B64">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C64">
+        <v>30</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 30 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B65">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C65">
+        <v>50</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 50 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B66">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C66">
+        <v>100</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 100 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B67">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C67">
+        <v>150</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D130" si="2">$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B67 &amp; " -v " &amp; C67 &amp; " &gt;&gt; logs/" &amp; B67 &amp; ".log 2&gt;&amp;1"</f>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 150 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C68">
+        <v>200</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 200 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B69">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C69">
+        <v>300</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 300 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B70">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C70">
+        <v>400</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 400 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B71">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C71">
+        <v>500</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 500 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C72">
+        <v>700</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 700 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="C73">
+        <v>1000</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 5000 -v 1000 &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B74">
+        <v>10000</v>
+      </c>
+      <c r="C74">
+        <v>10</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 10 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B75">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="C75">
+        <v>20</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 20 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B76">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="C76">
+        <v>30</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 30 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B77">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="C77">
+        <v>50</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 50 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B78">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="C78">
+        <v>100</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 100 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B79">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="C79">
+        <v>150</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 150 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B80">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="C80">
+        <v>200</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 200 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B81">
+        <f t="shared" ref="B81:B133" si="3">B80</f>
+        <v>10000</v>
+      </c>
+      <c r="C81">
+        <v>300</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 300 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B82">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+      <c r="C82">
+        <v>400</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 400 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B83">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+      <c r="C83">
+        <v>500</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 500 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B84">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+      <c r="C84">
+        <v>700</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 700 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B85">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+      <c r="C85">
+        <v>1000</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 10000 -v 1000 &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B86">
+        <v>20000</v>
+      </c>
+      <c r="C86">
+        <v>10</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 10 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B87">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C87">
+        <v>20</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 20 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B88">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C88">
+        <v>30</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 30 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B89">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C89">
+        <v>50</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 50 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B90">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C90">
+        <v>100</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 100 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B91">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C91">
+        <v>150</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 150 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B92">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C92">
+        <v>200</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 200 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B93">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C93">
+        <v>300</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 300 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B94">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C94">
+        <v>400</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 400 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B95">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C95">
+        <v>500</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 500 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B96">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C96">
+        <v>700</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 700 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B97">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="C97">
+        <v>1000</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 20000 -v 1000 &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B98">
+        <v>30000</v>
+      </c>
+      <c r="C98">
+        <v>10</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 10 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B99">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C99">
+        <v>20</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 20 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B100">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C100">
+        <v>30</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 30 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B101">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C101">
+        <v>50</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 50 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B102">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C102">
+        <v>100</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 100 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B103">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C103">
+        <v>150</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 150 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B104">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C104">
+        <v>200</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 200 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B105">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C105">
+        <v>300</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 300 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B106">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C106">
+        <v>400</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 400 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B107">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C107">
+        <v>500</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 500 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B108">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C108">
+        <v>700</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 700 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B109">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="C109">
+        <v>1000</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 30000 -v 1000 &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B110">
+        <v>40000</v>
+      </c>
+      <c r="C110">
+        <v>10</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 10 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B111">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="C111">
+        <v>20</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 20 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B112">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="C112">
+        <v>30</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 30 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B113">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="C113">
+        <v>50</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 50 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B114">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="C114">
+        <v>100</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 100 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B115">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="C115">
+        <v>150</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 150 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B116">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="C116">
+        <v>200</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 200 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B117">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="C117">
+        <v>300</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 300 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B118">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="C118">
+        <v>400</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 400 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B119">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="C119">
+        <v>500</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 500 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B120">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="C120">
+        <v>700</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 700 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B121">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
       <c r="C121">
         <v>1000</v>
       </c>
       <c r="D121" t="str">
-        <f t="shared" si="3"/>
-        <v>C:/Users/Pc/Documents/GitHub/241165/.venv/Scripts/python.exe c:/Users/Pc/Documents/GitHub/241165/run_batch.py -f 50000 -v 1000 &gt;&gt; logs\50000.log 2&gt;&amp;1</v>
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 40000 -v 1000 &gt;&gt; logs/40000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B122">
+        <v>50000</v>
+      </c>
+      <c r="C122">
+        <v>10</v>
+      </c>
+      <c r="D122" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 10 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B123">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C123">
+        <v>20</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 20 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B124">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C124">
+        <v>30</v>
+      </c>
+      <c r="D124" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 30 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B125">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C125">
+        <v>50</v>
+      </c>
+      <c r="D125" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 50 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B126">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C126">
+        <v>100</v>
+      </c>
+      <c r="D126" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 100 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B127">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C127">
+        <v>150</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 150 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B128">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C128">
+        <v>200</v>
+      </c>
+      <c r="D128" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 200 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B129">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C129">
+        <v>300</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 300 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B130">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C130">
+        <v>400</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" si="2"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 400 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B131">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C131">
+        <v>500</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" ref="D131:D132" si="4">$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B131 &amp; " -v " &amp; C131 &amp; " &gt;&gt; logs/" &amp; B131 &amp; ".log 2&gt;&amp;1"</f>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 500 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B132">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C132">
+        <v>700</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="4"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 700 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B133">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="C133">
+        <v>1000</v>
+      </c>
+      <c r="D133" t="str">
+        <f>$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B133 &amp; " -v " &amp; C133 &amp; " &gt;&gt; logs/" &amp; B133 &amp; ".log 2&gt;&amp;1"</f>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 50000 -v 1000 &gt;&gt; logs/50000.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA8C231-7267-4D05-BB1F-3592B555F2FF}">
+  <dimension ref="A1:T8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="8.62890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>2000</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" t="str">
+        <f>$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B2 &amp; " -v " &amp; C2 &amp; " -m " &amp; D2 &amp; " &gt;&gt; logs/" &amp; D2 &amp; ".log 2&gt;&amp;1"</f>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 100 -m 10 &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2000</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E8" si="0">$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B3 &amp; " -v " &amp; C3 &amp; " -m " &amp; D3 &amp; " &gt;&gt; logs/" &amp; D3 &amp; ".log 2&gt;&amp;1"</f>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 100 -m 20 &gt;&gt; logs/20.log 2&gt;&amp;1</v>
+      </c>
+      <c r="T3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4">
+        <v>2000</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 100 -m 30 &gt;&gt; logs/30.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5">
+        <v>2000</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 100 -m 40 &gt;&gt; logs/40.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6">
+        <v>2000</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 100 -m 50 &gt;&gt; logs/50.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7">
+        <v>2000</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 100 -m 100 &gt;&gt; logs/100.log 2&gt;&amp;1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8">
+        <v>2000</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_batch.py -f 2000 -v 100 -m 5 &gt;&gt; logs/5.log 2&gt;&amp;1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change batch file and multi parser
</commit_message>
<xml_diff>
--- a/runs.xlsx
+++ b/runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Documents\GitHub\241165\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E3FF4A-F5D2-4623-A020-40AFE85BDEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B325B8B8-4012-4407-9B81-CA048B357E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="3" xr2:uid="{88C63FDF-66B9-42B3-9B5D-45766DF4CCDF}"/>
+    <workbookView xWindow="63900" yWindow="4545" windowWidth="18900" windowHeight="10590" activeTab="3" xr2:uid="{88C63FDF-66B9-42B3-9B5D-45766DF4CCDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>File</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>/home/stimsim/Documents/241165/run_parser_multi.py</t>
+  </si>
+  <si>
+    <t>depth</t>
   </si>
 </sst>
 </file>
@@ -4057,7 +4060,7 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E2:E11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4078,6 +4081,9 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -4092,9 +4098,12 @@
       <c r="D2">
         <v>10</v>
       </c>
-      <c r="E2" t="str">
-        <f>$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B2 &amp; " -v " &amp; C2 &amp; " -m " &amp; D2 &amp; " -b &gt;&gt; logs/" &amp; D2 &amp; ".log 2&gt;&amp;1"</f>
-        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 2000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -b &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <f>$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B2 &amp; " -v " &amp; C2 &amp; " -m " &amp; D2 &amp; " -d " &amp; E2 &amp; " -b &gt;&gt; logs/" &amp; B2 &amp; ".log 2&gt;&amp;1"</f>
+        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 2000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -d 1 -b &gt;&gt; logs/2000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -4110,9 +4119,12 @@
       <c r="D3">
         <v>10</v>
       </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E11" si="0">$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B3 &amp; " -v " &amp; C3 &amp; " -m " &amp; D3 &amp; " -b &gt;&gt; logs/" &amp; D3 &amp; ".log 2&gt;&amp;1"</f>
-        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 4000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -b &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F11" si="0">$A$3 &amp; " " &amp; $A$2 &amp; " -f " &amp; B3 &amp; " -v " &amp; C3 &amp; " -m " &amp; D3 &amp; " -d " &amp; E3 &amp; " -b &gt;&gt; logs/" &amp; B3 &amp; ".log 2&gt;&amp;1"</f>
+        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 4000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -d 1 -b &gt;&gt; logs/4000.log 2&gt;&amp;1</v>
       </c>
       <c r="T3" t="s">
         <v>4</v>
@@ -4128,9 +4140,12 @@
       <c r="D4">
         <v>10</v>
       </c>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 5000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -b &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 5000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -d 1 -b &gt;&gt; logs/5000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -4143,9 +4158,12 @@
       <c r="D5">
         <v>10</v>
       </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 8000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -b &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 8000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -d 1 -b &gt;&gt; logs/8000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -4158,9 +4176,12 @@
       <c r="D6">
         <v>10</v>
       </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 10000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -b &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 10000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -d 1 -b &gt;&gt; logs/10000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -4173,9 +4194,12 @@
       <c r="D7">
         <v>10</v>
       </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 15000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -b &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 15000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -d 1 -b &gt;&gt; logs/15000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -4188,9 +4212,12 @@
       <c r="D8">
         <v>10</v>
       </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 20000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -b &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 20000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -d 1 -b &gt;&gt; logs/20000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -4203,9 +4230,12 @@
       <c r="D9">
         <v>10</v>
       </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 25000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -b &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 25000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -d 1 -b &gt;&gt; logs/25000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -4218,9 +4248,12 @@
       <c r="D10">
         <v>10</v>
       </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 30000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -b &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 30000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -d 1 -b &gt;&gt; logs/30000.log 2&gt;&amp;1</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -4233,9 +4266,12 @@
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 35000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -b &gt;&gt; logs/10.log 2&gt;&amp;1</v>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>python3 /home/stimsim/Documents/241165/run_parser_multi.py -f 35000 -v 1 2 3 5 10 15 20 30 40 50 70 100 200 -m 10 -d 1 -b &gt;&gt; logs/35000.log 2&gt;&amp;1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>